<commit_message>
Requirements phase reviewed and changed
</commit_message>
<xml_diff>
--- a/01_Tasks/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/01_Tasks/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\01_Tasks\01_Tasks\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3869105-1D24-4AFE-94B6-A2A2B4E76E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AC54FF-275F-43CB-A0C4-1647B466EBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="44">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -159,19 +159,35 @@
   </si>
   <si>
     <t>Nu se furnizeaza detalii arhitecturale /  de platforma</t>
+  </si>
+  <si>
+    <t>Petrila Claudiu-Nicolae</t>
+  </si>
+  <si>
+    <t>Muresan Victor-Andrei</t>
+  </si>
+  <si>
+    <t>Popovici George-Octavian</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -350,79 +366,80 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,8 +749,8 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,7 +760,7 @@
     <col min="3" max="4" width="16.21875" style="6" customWidth="1"/>
     <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
     <col min="6" max="8" width="8.88671875" style="6"/>
-    <col min="9" max="9" width="21" style="6" customWidth="1"/>
+    <col min="9" max="9" width="22.44140625" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.44140625" style="6" customWidth="1"/>
     <col min="11" max="16384" width="8.88671875" style="6"/>
   </cols>
@@ -778,8 +795,12 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="I3" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="17">
+        <v>235</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="13" t="s">
@@ -792,8 +813,12 @@
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="3">
+        <v>235</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="13" t="s">
@@ -806,8 +831,12 @@
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="3">
+        <v>235</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
@@ -838,40 +867,64 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
+      <c r="C13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
@@ -880,7 +933,7 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="2"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
@@ -889,7 +942,7 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
@@ -986,7 +1039,9 @@
         <v>8</v>
       </c>
       <c r="D27" s="12"/>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1295,7 +1350,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1616,8 +1671,8 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1663,8 +1718,12 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="I3" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="17">
+        <v>235</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="16" t="s">
@@ -1675,8 +1734,12 @@
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="3">
+        <v>235</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="9" t="s">
@@ -1687,8 +1750,12 @@
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="3">
+        <v>235</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
@@ -1716,68 +1783,44 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">

</xml_diff>

<commit_message>
Updated Excel and modified with Sonar recommendations
</commit_message>
<xml_diff>
--- a/01_Tasks/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/01_Tasks/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\01_Tasks\01_Tasks\Docs\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\popov\OneDrive\Desktop\VVSS_Tasks\01_Tasks\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24714B4F-6DEA-4C38-9F7B-A3A78D55E7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76012192-789A-4CC5-B94D-71CCB26101A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="76">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -134,9 +134,6 @@
     <t>Tool-based Code Analysis</t>
   </si>
   <si>
-    <t>Effort to perform tool-based code analysis (hours):</t>
-  </si>
-  <si>
     <t>R04</t>
   </si>
   <si>
@@ -201,6 +198,91 @@
   </si>
   <si>
     <t>Nu avem nume la agregari/ asocieri</t>
+  </si>
+  <si>
+    <t>Popovici George Octavian</t>
+  </si>
+  <si>
+    <t>Effort to perform tool-based code analysis (hours): 0.5 hour</t>
+  </si>
+  <si>
+    <t>Instance methods should not write to "static" fields</t>
+  </si>
+  <si>
+    <t>Controller.Java, 22</t>
+  </si>
+  <si>
+    <t>private Stage infoStage;     // ⬅️ Changed from static to instance variable</t>
+  </si>
+  <si>
+    <t>(139,28) Remove this "clone" implementation; use a copy constructor or copy factory instead</t>
+  </si>
+  <si>
+    <t>protected ArrayTaskList clone() throws CloneNotSupportedException {
+    ArrayTaskList tasks = new ArrayTaskList();
+    for (int i = 0; i &lt; this.tasks.length; i++){
+        tasks.add(this.getTask(i));
+    }
+    return tasks;
+}</t>
+  </si>
+  <si>
+    <t>ArrayTaskList.java, 139</t>
+  </si>
+  <si>
+    <t>Constant names should comply with a naming convention</t>
+  </si>
+  <si>
+    <t>Calendar calendar = GregorianCalendar.getInstance();</t>
+  </si>
+  <si>
+    <t>Called the method from the original class, as it's not overriden:
+Calendar calendar = Calendar.getInstance();</t>
+  </si>
+  <si>
+    <t>DateService.java, 41</t>
+  </si>
+  <si>
+    <t>private static final int defaultWidth = 820;</t>
+  </si>
+  <si>
+    <t>private static final int DEFAULT_WIDTH = 820;</t>
+  </si>
+  <si>
+    <t>private static final int defaultHeight = 520;</t>
+  </si>
+  <si>
+    <t>Main.Java,21</t>
+  </si>
+  <si>
+    <t>Main.Java,22</t>
+  </si>
+  <si>
+    <t>private static final int DEFAULT_WIDTH = 520;</t>
+  </si>
+  <si>
+    <t>"static" base class members should not be accessed via derived types</t>
+  </si>
+  <si>
+    <t>DateService.java 34</t>
+  </si>
+  <si>
+    <t>// Factory Method for Copying
+public static ArrayTaskList copyOf(ArrayTaskList other) {
+    ArrayTaskList copy = new ArrayTaskList();
+    copy.currentCapacity = other.currentCapacity;
+    copy.numberOfTasks = other.numberOfTasks;
+    copy.tasks = new Task[copy.currentCapacity];
+    for (int i = 0; i &lt; copy.numberOfTasks; i++) {
+        copy.tasks[i] = other.tasks[i]; // Shallow copy (modify for deep copy if needed)
+    }
+    return copy;
+}       
+ The clone() method was replaced with a factory method (copyOf()), which is the preferred approach.  
+ This allows ArrayTaskList.copyOf(original) instead of using clone().</t>
+  </si>
+  <si>
+    <t>public static Stage infoStage</t>
   </si>
 </sst>
 </file>
@@ -399,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -430,6 +512,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -469,10 +552,22 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,6 +583,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>478043</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>57814</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagine 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AF6D3D3-40F3-CD27-E553-6A7B0DD9B269}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="605118" y="12774706"/>
+          <a:ext cx="13738411" cy="7584357"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9298</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>169769</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>102232</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>91141</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagine 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1E56CA6-93FA-AEF6-1440-4E14684010D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="614416" y="23769357"/>
+          <a:ext cx="13349492" cy="6913843"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -803,19 +991,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -828,8 +1016,8 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="36" t="s">
-        <v>41</v>
+      <c r="I3" s="22" t="s">
+        <v>40</v>
       </c>
       <c r="J3" s="17">
         <v>235</v>
@@ -839,15 +1027,15 @@
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="26"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="36" t="s">
-        <v>42</v>
+      <c r="I4" s="22" t="s">
+        <v>41</v>
       </c>
       <c r="J4" s="3">
         <v>235</v>
@@ -857,15 +1045,15 @@
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="28"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="36" t="s">
-        <v>43</v>
+      <c r="I5" s="22" t="s">
+        <v>42</v>
       </c>
       <c r="J5" s="3">
         <v>235</v>
@@ -876,15 +1064,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -905,13 +1093,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -920,13 +1108,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -935,13 +1123,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -950,13 +1138,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1117,19 +1305,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1142,8 +1330,8 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="36" t="s">
-        <v>41</v>
+      <c r="I3" s="22" t="s">
+        <v>40</v>
       </c>
       <c r="J3" s="17">
         <v>235</v>
@@ -1153,15 +1341,15 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="29"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="36" t="s">
-        <v>42</v>
+      <c r="I4" s="22" t="s">
+        <v>41</v>
       </c>
       <c r="J4" s="3">
         <v>235</v>
@@ -1171,15 +1359,15 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="31"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="36" t="s">
-        <v>43</v>
+      <c r="I5" s="22" t="s">
+        <v>42</v>
       </c>
       <c r="J5" s="3">
         <v>235</v>
@@ -1190,15 +1378,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1219,13 +1407,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1234,13 +1422,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1249,13 +1437,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1264,13 +1452,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1279,13 +1467,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="E14" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1426,7 +1614,7 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1447,19 +1635,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1472,8 +1660,8 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="36" t="s">
-        <v>41</v>
+      <c r="I3" s="22" t="s">
+        <v>40</v>
       </c>
       <c r="J3" s="17">
         <v>235</v>
@@ -1483,15 +1671,15 @@
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="32"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="36" t="s">
-        <v>42</v>
+      <c r="I4" s="22" t="s">
+        <v>41</v>
       </c>
       <c r="J4" s="3">
         <v>235</v>
@@ -1501,15 +1689,15 @@
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="34"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="36" t="s">
-        <v>43</v>
+      <c r="I5" s="22" t="s">
+        <v>42</v>
       </c>
       <c r="J5" s="3">
         <v>235</v>
@@ -1520,15 +1708,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1760,8 +1948,8 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:E4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1782,19 +1970,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1807,8 +1995,8 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="36" t="s">
-        <v>41</v>
+      <c r="I3" s="22" t="s">
+        <v>40</v>
       </c>
       <c r="J3" s="17">
         <v>235</v>
@@ -1818,13 +2006,13 @@
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="36" t="s">
-        <v>42</v>
+      <c r="I4" s="22" t="s">
+        <v>41</v>
       </c>
       <c r="J4" s="3">
         <v>235</v>
@@ -1834,13 +2022,15 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
+      <c r="D5" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="23"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="36" t="s">
-        <v>43</v>
+      <c r="I5" s="22" t="s">
+        <v>42</v>
       </c>
       <c r="J5" s="3">
         <v>235</v>
@@ -1851,8 +2041,10 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="36">
+        <v>45731</v>
+      </c>
+      <c r="E6" s="23"/>
       <c r="F6" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1876,60 +2068,108 @@
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C11" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C12" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="409.6" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="C15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
@@ -2082,11 +2322,11 @@
       <c r="F30" s="2"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
+      <c r="C32" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
       <c r="F32" s="18"/>
     </row>
     <row r="35" spans="6:6" x14ac:dyDescent="0.3">
@@ -2103,5 +2343,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>